<commit_message>
Updates to latest 4.0
</commit_message>
<xml_diff>
--- a/InputData/ccs/BwCCSSpM/Biomass with CCS Storage per MWh.xlsx
+++ b/InputData/ccs/BwCCSSpM/Biomass with CCS Storage per MWh.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="27031"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="26626"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
@@ -16,20 +16,14 @@
     <sheet name="About" sheetId="1" r:id="rId1"/>
     <sheet name="BwCCSSpM" sheetId="12" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="191028"/>
+  <calcPr calcId="191029"/>
   <extLst>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
-      <x15:workbookPr chartTrackingRefBase="1"/>
-    </ext>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
         <xcalcf:feature name="microsoft.com:RD"/>
         <xcalcf:feature name="microsoft.com:Single"/>
         <xcalcf:feature name="microsoft.com:FV"/>
         <xcalcf:feature name="microsoft.com:CNMTM"/>
-        <xcalcf:feature name="microsoft.com:LET_WF"/>
-        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
-        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -39,25 +33,25 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="12">
   <si>
+    <t>Source:</t>
+  </si>
+  <si>
+    <t>Notes</t>
+  </si>
+  <si>
+    <t>Section 2.1.7</t>
+  </si>
+  <si>
+    <t>Donnison et al.</t>
+  </si>
+  <si>
+    <t>Bioenergy with Carbon Capture and Storage (BECCS): Finding the win-wins for energy, negative emissions and ecosystem services - size matters</t>
+  </si>
+  <si>
+    <t>https://onlinelibrary.wiley.com/doi/full/10.1111/gcbb.12695</t>
+  </si>
+  <si>
     <t>BwCCSSpM Biomass with CCS Storage per MWh</t>
-  </si>
-  <si>
-    <t>Source:</t>
-  </si>
-  <si>
-    <t>Donnison et al.</t>
-  </si>
-  <si>
-    <t>Bioenergy with Carbon Capture and Storage (BECCS): Finding the win-wins for energy, negative emissions and ecosystem services - size matters</t>
-  </si>
-  <si>
-    <t>https://onlinelibrary.wiley.com/doi/full/10.1111/gcbb.12695</t>
-  </si>
-  <si>
-    <t>Section 2.1.7</t>
-  </si>
-  <si>
-    <t>Notes</t>
   </si>
   <si>
     <t>Because the emissions intensity (see file fuels/PEI) of BECCS plants is often reported as 0, we need to separately specify here the</t>
@@ -79,7 +73,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -133,7 +127,7 @@
     </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Standard" xfId="0" builtinId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -446,7 +440,7 @@
       <selection activeCell="B14" sqref="B14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="2" max="2" width="103.42578125" customWidth="1"/>
     <col min="3" max="3" width="17.140625" customWidth="1"/>
@@ -454,55 +448,55 @@
     <col min="5" max="5" width="18.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3" s="1" t="s">
         <v>0</v>
       </c>
-    </row>
-    <row r="3" spans="1:2">
-      <c r="A3" s="1" t="s">
-        <v>1</v>
-      </c>
       <c r="B3" s="3" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B4" s="3">
         <v>2020</v>
       </c>
     </row>
-    <row r="5" spans="1:2">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B5" s="3" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="6" spans="1:2">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B6" s="3" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="7" spans="1:2">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B7" s="3" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="9" spans="1:2">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="10" spans="1:2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="11" spans="1:2">
+    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="12" spans="1:2">
+    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>9</v>
       </c>
@@ -524,18 +518,18 @@
       <selection activeCell="D29" sqref="D29"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="30.140625" customWidth="1"/>
     <col min="2" max="2" width="11" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B1" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="2" spans="1:2">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
         <v>11</v>
       </c>
@@ -548,259 +542,4 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
-</file>
-
-<file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100A08BDF573E2FFD46A5F05DED9AF68025" ma:contentTypeVersion="13" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="f85c0eb68479ad8b8987805fd5b8836b">
-  <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="00484652-42e1-479e-92f4-fb0efddcdf60" xmlns:ns3="41b1c9bf-5b6b-463b-ba12-a3b9bfbff0d3" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="f7dbc72841229da9eaa30ebb1456cd70" ns2:_="" ns3:_="">
-    <xsd:import namespace="00484652-42e1-479e-92f4-fb0efddcdf60"/>
-    <xsd:import namespace="41b1c9bf-5b6b-463b-ba12-a3b9bfbff0d3"/>
-    <xsd:element name="properties">
-      <xsd:complexType>
-        <xsd:sequence>
-          <xsd:element name="documentManagement">
-            <xsd:complexType>
-              <xsd:all>
-                <xsd:element ref="ns2:MediaServiceMetadata" minOccurs="0"/>
-                <xsd:element ref="ns2:MediaServiceFastMetadata" minOccurs="0"/>
-                <xsd:element ref="ns2:MediaServiceObjectDetectorVersions" minOccurs="0"/>
-                <xsd:element ref="ns2:lcf76f155ced4ddcb4097134ff3c332f" minOccurs="0"/>
-                <xsd:element ref="ns3:TaxCatchAll" minOccurs="0"/>
-                <xsd:element ref="ns2:MediaServiceGenerationTime" minOccurs="0"/>
-                <xsd:element ref="ns2:MediaServiceEventHashCode" minOccurs="0"/>
-                <xsd:element ref="ns2:MediaServiceDateTaken" minOccurs="0"/>
-                <xsd:element ref="ns2:MediaServiceLocation" minOccurs="0"/>
-                <xsd:element ref="ns2:MediaServiceOCR" minOccurs="0"/>
-                <xsd:element ref="ns3:SharedWithUsers" minOccurs="0"/>
-                <xsd:element ref="ns3:SharedWithDetails" minOccurs="0"/>
-              </xsd:all>
-            </xsd:complexType>
-          </xsd:element>
-        </xsd:sequence>
-      </xsd:complexType>
-    </xsd:element>
-  </xsd:schema>
-  <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:dms="http://schemas.microsoft.com/office/2006/documentManagement/types" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls" targetNamespace="00484652-42e1-479e-92f4-fb0efddcdf60" elementFormDefault="qualified">
-    <xsd:import namespace="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <xsd:import namespace="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <xsd:element name="MediaServiceMetadata" ma:index="8" nillable="true" ma:displayName="MediaServiceMetadata" ma:hidden="true" ma:internalName="MediaServiceMetadata" ma:readOnly="true">
-      <xsd:simpleType>
-        <xsd:restriction base="dms:Note"/>
-      </xsd:simpleType>
-    </xsd:element>
-    <xsd:element name="MediaServiceFastMetadata" ma:index="9" nillable="true" ma:displayName="MediaServiceFastMetadata" ma:hidden="true" ma:internalName="MediaServiceFastMetadata" ma:readOnly="true">
-      <xsd:simpleType>
-        <xsd:restriction base="dms:Note"/>
-      </xsd:simpleType>
-    </xsd:element>
-    <xsd:element name="MediaServiceObjectDetectorVersions" ma:index="10" nillable="true" ma:displayName="MediaServiceObjectDetectorVersions" ma:hidden="true" ma:indexed="true" ma:internalName="MediaServiceObjectDetectorVersions" ma:readOnly="true">
-      <xsd:simpleType>
-        <xsd:restriction base="dms:Text"/>
-      </xsd:simpleType>
-    </xsd:element>
-    <xsd:element name="lcf76f155ced4ddcb4097134ff3c332f" ma:index="12" nillable="true" ma:taxonomy="true" ma:internalName="lcf76f155ced4ddcb4097134ff3c332f" ma:taxonomyFieldName="MediaServiceImageTags" ma:displayName="Image Tags" ma:readOnly="false" ma:fieldId="{5cf76f15-5ced-4ddc-b409-7134ff3c332f}" ma:taxonomyMulti="true" ma:sspId="eca5b831-c3dc-41cf-bd85-218b82cecb21" ma:termSetId="09814cd3-568e-fe90-9814-8d621ff8fb84" ma:anchorId="fba54fb3-c3e1-fe81-a776-ca4b69148c4d" ma:open="true" ma:isKeyword="false">
-      <xsd:complexType>
-        <xsd:sequence>
-          <xsd:element ref="pc:Terms" minOccurs="0" maxOccurs="1"/>
-        </xsd:sequence>
-      </xsd:complexType>
-    </xsd:element>
-    <xsd:element name="MediaServiceGenerationTime" ma:index="14" nillable="true" ma:displayName="MediaServiceGenerationTime" ma:hidden="true" ma:internalName="MediaServiceGenerationTime" ma:readOnly="true">
-      <xsd:simpleType>
-        <xsd:restriction base="dms:Text"/>
-      </xsd:simpleType>
-    </xsd:element>
-    <xsd:element name="MediaServiceEventHashCode" ma:index="15" nillable="true" ma:displayName="MediaServiceEventHashCode" ma:hidden="true" ma:internalName="MediaServiceEventHashCode" ma:readOnly="true">
-      <xsd:simpleType>
-        <xsd:restriction base="dms:Text"/>
-      </xsd:simpleType>
-    </xsd:element>
-    <xsd:element name="MediaServiceDateTaken" ma:index="16" nillable="true" ma:displayName="MediaServiceDateTaken" ma:hidden="true" ma:indexed="true" ma:internalName="MediaServiceDateTaken" ma:readOnly="true">
-      <xsd:simpleType>
-        <xsd:restriction base="dms:Text"/>
-      </xsd:simpleType>
-    </xsd:element>
-    <xsd:element name="MediaServiceLocation" ma:index="17" nillable="true" ma:displayName="Location" ma:indexed="true" ma:internalName="MediaServiceLocation" ma:readOnly="true">
-      <xsd:simpleType>
-        <xsd:restriction base="dms:Text"/>
-      </xsd:simpleType>
-    </xsd:element>
-    <xsd:element name="MediaServiceOCR" ma:index="18" nillable="true" ma:displayName="Extracted Text" ma:internalName="MediaServiceOCR" ma:readOnly="true">
-      <xsd:simpleType>
-        <xsd:restriction base="dms:Note">
-          <xsd:maxLength value="255"/>
-        </xsd:restriction>
-      </xsd:simpleType>
-    </xsd:element>
-  </xsd:schema>
-  <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:dms="http://schemas.microsoft.com/office/2006/documentManagement/types" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls" targetNamespace="41b1c9bf-5b6b-463b-ba12-a3b9bfbff0d3" elementFormDefault="qualified">
-    <xsd:import namespace="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <xsd:import namespace="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <xsd:element name="TaxCatchAll" ma:index="13" nillable="true" ma:displayName="Taxonomy Catch All Column" ma:hidden="true" ma:list="{c5b79d03-3bfd-4c46-9947-056a2403f6c9}" ma:internalName="TaxCatchAll" ma:showField="CatchAllData" ma:web="41b1c9bf-5b6b-463b-ba12-a3b9bfbff0d3">
-      <xsd:complexType>
-        <xsd:complexContent>
-          <xsd:extension base="dms:MultiChoiceLookup">
-            <xsd:sequence>
-              <xsd:element name="Value" type="dms:Lookup" maxOccurs="unbounded" minOccurs="0" nillable="true"/>
-            </xsd:sequence>
-          </xsd:extension>
-        </xsd:complexContent>
-      </xsd:complexType>
-    </xsd:element>
-    <xsd:element name="SharedWithUsers" ma:index="19" nillable="true" ma:displayName="Shared With" ma:internalName="SharedWithUsers" ma:readOnly="true">
-      <xsd:complexType>
-        <xsd:complexContent>
-          <xsd:extension base="dms:UserMulti">
-            <xsd:sequence>
-              <xsd:element name="UserInfo" minOccurs="0" maxOccurs="unbounded">
-                <xsd:complexType>
-                  <xsd:sequence>
-                    <xsd:element name="DisplayName" type="xsd:string" minOccurs="0"/>
-                    <xsd:element name="AccountId" type="dms:UserId" minOccurs="0" nillable="true"/>
-                    <xsd:element name="AccountType" type="xsd:string" minOccurs="0"/>
-                  </xsd:sequence>
-                </xsd:complexType>
-              </xsd:element>
-            </xsd:sequence>
-          </xsd:extension>
-        </xsd:complexContent>
-      </xsd:complexType>
-    </xsd:element>
-    <xsd:element name="SharedWithDetails" ma:index="20" nillable="true" ma:displayName="Shared With Details" ma:internalName="SharedWithDetails" ma:readOnly="true">
-      <xsd:simpleType>
-        <xsd:restriction base="dms:Note">
-          <xsd:maxLength value="255"/>
-        </xsd:restriction>
-      </xsd:simpleType>
-    </xsd:element>
-  </xsd:schema>
-  <xsd:schema xmlns="http://schemas.openxmlformats.org/package/2006/metadata/core-properties" xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:dc="http://purl.org/dc/elements/1.1/" xmlns:dcterms="http://purl.org/dc/terms/" xmlns:odoc="http://schemas.microsoft.com/internal/obd" targetNamespace="http://schemas.openxmlformats.org/package/2006/metadata/core-properties" elementFormDefault="qualified" attributeFormDefault="unqualified" blockDefault="#all">
-    <xsd:import namespace="http://purl.org/dc/elements/1.1/" schemaLocation="http://dublincore.org/schemas/xmls/qdc/2003/04/02/dc.xsd"/>
-    <xsd:import namespace="http://purl.org/dc/terms/" schemaLocation="http://dublincore.org/schemas/xmls/qdc/2003/04/02/dcterms.xsd"/>
-    <xsd:element name="coreProperties" type="CT_coreProperties"/>
-    <xsd:complexType name="CT_coreProperties">
-      <xsd:all>
-        <xsd:element ref="dc:creator" minOccurs="0" maxOccurs="1"/>
-        <xsd:element ref="dcterms:created" minOccurs="0" maxOccurs="1"/>
-        <xsd:element ref="dc:identifier" minOccurs="0" maxOccurs="1"/>
-        <xsd:element name="contentType" minOccurs="0" maxOccurs="1" type="xsd:string" ma:index="0" ma:displayName="Content Type"/>
-        <xsd:element ref="dc:title" minOccurs="0" maxOccurs="1" ma:index="4" ma:displayName="Title"/>
-        <xsd:element ref="dc:subject" minOccurs="0" maxOccurs="1"/>
-        <xsd:element ref="dc:description" minOccurs="0" maxOccurs="1"/>
-        <xsd:element name="keywords" minOccurs="0" maxOccurs="1" type="xsd:string"/>
-        <xsd:element ref="dc:language" minOccurs="0" maxOccurs="1"/>
-        <xsd:element name="category" minOccurs="0" maxOccurs="1" type="xsd:string"/>
-        <xsd:element name="version" minOccurs="0" maxOccurs="1" type="xsd:string"/>
-        <xsd:element name="revision" minOccurs="0" maxOccurs="1" type="xsd:string">
-          <xsd:annotation>
-            <xsd:documentation>
-                        This value indicates the number of saves or revisions. The application is responsible for updating this value after each revision.
-                    </xsd:documentation>
-          </xsd:annotation>
-        </xsd:element>
-        <xsd:element name="lastModifiedBy" minOccurs="0" maxOccurs="1" type="xsd:string"/>
-        <xsd:element ref="dcterms:modified" minOccurs="0" maxOccurs="1"/>
-        <xsd:element name="contentStatus" minOccurs="0" maxOccurs="1" type="xsd:string"/>
-      </xsd:all>
-    </xsd:complexType>
-  </xsd:schema>
-  <xs:schema xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls" xmlns:xs="http://www.w3.org/2001/XMLSchema" targetNamespace="http://schemas.microsoft.com/office/infopath/2007/PartnerControls" elementFormDefault="qualified" attributeFormDefault="unqualified">
-    <xs:element name="Person">
-      <xs:complexType>
-        <xs:sequence>
-          <xs:element ref="pc:DisplayName" minOccurs="0"/>
-          <xs:element ref="pc:AccountId" minOccurs="0"/>
-          <xs:element ref="pc:AccountType" minOccurs="0"/>
-        </xs:sequence>
-      </xs:complexType>
-    </xs:element>
-    <xs:element name="DisplayName" type="xs:string"/>
-    <xs:element name="AccountId" type="xs:string"/>
-    <xs:element name="AccountType" type="xs:string"/>
-    <xs:element name="BDCAssociatedEntity">
-      <xs:complexType>
-        <xs:sequence>
-          <xs:element ref="pc:BDCEntity" minOccurs="0" maxOccurs="unbounded"/>
-        </xs:sequence>
-        <xs:attribute ref="pc:EntityNamespace"/>
-        <xs:attribute ref="pc:EntityName"/>
-        <xs:attribute ref="pc:SystemInstanceName"/>
-        <xs:attribute ref="pc:AssociationName"/>
-      </xs:complexType>
-    </xs:element>
-    <xs:attribute name="EntityNamespace" type="xs:string"/>
-    <xs:attribute name="EntityName" type="xs:string"/>
-    <xs:attribute name="SystemInstanceName" type="xs:string"/>
-    <xs:attribute name="AssociationName" type="xs:string"/>
-    <xs:element name="BDCEntity">
-      <xs:complexType>
-        <xs:sequence>
-          <xs:element ref="pc:EntityDisplayName" minOccurs="0"/>
-          <xs:element ref="pc:EntityInstanceReference" minOccurs="0"/>
-          <xs:element ref="pc:EntityId1" minOccurs="0"/>
-          <xs:element ref="pc:EntityId2" minOccurs="0"/>
-          <xs:element ref="pc:EntityId3" minOccurs="0"/>
-          <xs:element ref="pc:EntityId4" minOccurs="0"/>
-          <xs:element ref="pc:EntityId5" minOccurs="0"/>
-        </xs:sequence>
-      </xs:complexType>
-    </xs:element>
-    <xs:element name="EntityDisplayName" type="xs:string"/>
-    <xs:element name="EntityInstanceReference" type="xs:string"/>
-    <xs:element name="EntityId1" type="xs:string"/>
-    <xs:element name="EntityId2" type="xs:string"/>
-    <xs:element name="EntityId3" type="xs:string"/>
-    <xs:element name="EntityId4" type="xs:string"/>
-    <xs:element name="EntityId5" type="xs:string"/>
-    <xs:element name="Terms">
-      <xs:complexType>
-        <xs:sequence>
-          <xs:element ref="pc:TermInfo" minOccurs="0" maxOccurs="unbounded"/>
-        </xs:sequence>
-      </xs:complexType>
-    </xs:element>
-    <xs:element name="TermInfo">
-      <xs:complexType>
-        <xs:sequence>
-          <xs:element ref="pc:TermName" minOccurs="0"/>
-          <xs:element ref="pc:TermId" minOccurs="0"/>
-        </xs:sequence>
-      </xs:complexType>
-    </xs:element>
-    <xs:element name="TermName" type="xs:string"/>
-    <xs:element name="TermId" type="xs:string"/>
-  </xs:schema>
-</ct:contentTypeSchema>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="00484652-42e1-479e-92f4-fb0efddcdf60">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-    <TaxCatchAll xmlns="41b1c9bf-5b6b-463b-ba12-a3b9bfbff0d3" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{0A6F04A0-CEC6-4BCD-9A31-0348F244D45A}"/>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{5C826B88-A8CF-4CB1-990D-B89E049A1CCF}"/>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{C5A267F7-8CC2-482F-A950-B9D3B1D451AE}"/>
 </file>
</xml_diff>